<commit_message>
Fixed small issue in paraser, evaluation of finnish output, reevaluation of english output. Added utility to compare hits result between 2 languages (effectively generating JSONS with entries where lang1 performed bbetter than lang2, performed equally good and lang2 performing better than lang1)
</commit_message>
<xml_diff>
--- a/outputs/hits_k_excel/hits_k_zeroshot_da.xlsx
+++ b/outputs/hits_k_excel/hits_k_zeroshot_da.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lasse\Documents\6sem\Project\extended-mintaka\outputs\hits_k_excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4328FF2E-B230-453E-B391-FAD4DE89FE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Total Hits"/>
-    <sheet r:id="rId2" sheetId="2" name="Hits_boolean"/>
-    <sheet r:id="rId3" sheetId="3" name="Hits_entity"/>
-    <sheet r:id="rId4" sheetId="4" name="Hits_numerical"/>
-    <sheet r:id="rId5" sheetId="5" name="Hits_date"/>
-    <sheet r:id="rId6" sheetId="6" name="Hits_string"/>
+    <sheet name="Total Hits" sheetId="1" r:id="rId1"/>
+    <sheet name="Hits_boolean" sheetId="2" r:id="rId2"/>
+    <sheet name="Hits_entity" sheetId="3" r:id="rId3"/>
+    <sheet name="Hits_numerical" sheetId="4" r:id="rId4"/>
+    <sheet name="Hits_date" sheetId="5" r:id="rId5"/>
+    <sheet name="Hits_string" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -126,8 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,32 +175,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -206,10 +205,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -247,71 +246,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -339,7 +338,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -362,11 +361,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -375,13 +374,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -391,7 +390,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -400,7 +399,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -409,7 +408,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -417,10 +416,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -485,7 +484,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -493,15 +492,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,77 +508,77 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>2201</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>3612</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>4428</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>7224</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>6652</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>10836</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>8888</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>14448</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>11088</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>18060</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -591,113 +588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>398</v>
-      </c>
-      <c r="C2" s="3">
-        <v>573</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>786</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1146</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1173</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1719</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1567</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2292</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1962</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2865</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -705,15 +596,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,78 +612,78 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>1273</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2111</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
+      <c r="B2" s="2">
+        <v>398</v>
+      </c>
+      <c r="C2" s="2">
+        <v>573</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>2585</v>
-      </c>
-      <c r="C3" s="3">
-        <v>4222</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
+      <c r="B3" s="2">
+        <v>786</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1146</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>3873</v>
-      </c>
-      <c r="C4" s="3">
-        <v>6333</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
+      <c r="B4" s="2">
+        <v>1173</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1719</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>5168</v>
-      </c>
-      <c r="C5" s="3">
-        <v>8444</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
+      <c r="B5" s="2">
+        <v>1567</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2292</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>6442</v>
-      </c>
-      <c r="C6" s="3">
-        <v>10555</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
+      <c r="B6" s="2">
+        <v>1962</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2865</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -802,8 +691,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -811,15 +700,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,78 +716,78 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>340</v>
-      </c>
-      <c r="C2" s="3">
-        <v>655</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
+      <c r="B2" s="2">
+        <v>1273</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>679</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1310</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
+      <c r="B3" s="2">
+        <v>2585</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4222</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>1037</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1965</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
+      <c r="B4" s="2">
+        <v>3873</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6333</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>1394</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2620</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
+      <c r="B5" s="2">
+        <v>5168</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8444</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>1738</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3275</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
+      <c r="B6" s="2">
+        <v>6442</v>
+      </c>
+      <c r="C6" s="2">
+        <v>10555</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -908,8 +795,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -917,15 +804,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,77 +820,183 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
+        <v>340</v>
+      </c>
+      <c r="C2" s="2">
+        <v>655</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>679</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1310</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1037</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1965</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1394</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2620</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1738</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3275</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
         <v>183</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>265</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>365</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>530</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>550</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>795</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>734</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1060</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>913</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1325</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1015,7 +1006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1023,15 +1014,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1041,77 +1030,77 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>13</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>19</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>25</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>32</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>33</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>40</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>